<commit_message>
test for multiple donations per cost item
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@67108 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/project/contributions.xlsx
+++ b/RIV4-tests/src/test/resources/imports/project/contributions.xlsx
@@ -122,30 +122,25 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -159,27 +154,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t/>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4.0</v>
       </c>
       <c r="E5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F5" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G5" s="5">
-        <f>E5*F5</f>
+      <c r="F5" s="5">
+        <f>D5*E5</f>
         <v>0.0</v>
       </c>
     </row>
@@ -191,38 +181,33 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t/>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1.0</v>
       </c>
       <c r="E6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="5">
-        <f>E6*F6</f>
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="5">
+        <f>D6*E6</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="F7" s="2" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G7" s="5">
-        <f>SUM(G5:G6)</f>
+      <c r="F7" s="5">
+        <f>SUM(F5:F6)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -241,30 +226,25 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -278,27 +258,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t/>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.0</v>
       </c>
       <c r="E11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F11" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G11" s="5">
-        <f>E11*F11</f>
+      <c r="F11" s="5">
+        <f>D11*E11</f>
         <v>0.0</v>
       </c>
     </row>
@@ -310,38 +285,33 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t/>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1.0</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G12" s="5">
-        <f>E12*F12</f>
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="5">
+        <f>D12*E12</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="F13" s="2" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G13" s="5">
-        <f>SUM(G11:G12)</f>
+      <c r="F13" s="5">
+        <f>SUM(F11:F12)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -360,30 +330,25 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G16" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -397,27 +362,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.0</v>
       </c>
       <c r="E17" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F17" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G17" s="5">
-        <f>E17*F17</f>
+      <c r="F17" s="5">
+        <f>D17*E17</f>
         <v>0.0</v>
       </c>
     </row>
@@ -429,38 +389,33 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.0</v>
       </c>
       <c r="E18" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="5">
-        <f>E18*F18</f>
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="5">
+        <f>D18*E18</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="F19" s="2" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G19" s="5">
-        <f>SUM(G17:G18)</f>
+      <c r="F19" s="5">
+        <f>SUM(F17:F18)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -479,30 +434,25 @@
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G22" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -516,27 +466,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.0</v>
       </c>
       <c r="E23" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F23" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G23" s="5">
-        <f>E23*F23</f>
+      <c r="F23" s="5">
+        <f>D23*E23</f>
         <v>0.0</v>
       </c>
     </row>
@@ -548,38 +493,33 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1.0</v>
       </c>
       <c r="E24" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G24" s="5">
-        <f>E24*F24</f>
+        <v>0.0</v>
+      </c>
+      <c r="F24" s="5">
+        <f>D24*E24</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="F25" s="2" t="inlineStr">
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G25" s="5">
-        <f>SUM(G23:G24)</f>
+      <c r="F25" s="5">
+        <f>SUM(F23:F24)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -598,30 +538,25 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G28" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -635,27 +570,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.0</v>
       </c>
       <c r="E29" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F29" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G29" s="5">
-        <f>E29*F29</f>
+      <c r="F29" s="5">
+        <f>D29*E29</f>
         <v>0.0</v>
       </c>
     </row>
@@ -667,38 +597,33 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.0</v>
       </c>
       <c r="E30" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G30" s="5">
-        <f>E30*F30</f>
+        <v>0.0</v>
+      </c>
+      <c r="F30" s="5">
+        <f>D30*E30</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="31">
-      <c r="F31" s="2" t="inlineStr">
+      <c r="E31" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G31" s="5">
-        <f>SUM(G29:G30)</f>
+      <c r="F31" s="5">
+        <f>SUM(F29:F30)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -717,30 +642,25 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F34" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G34" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -754,27 +674,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.0</v>
       </c>
       <c r="E35" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F35" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G35" s="5">
-        <f>E35*F35</f>
+      <c r="F35" s="5">
+        <f>D35*E35</f>
         <v>0.0</v>
       </c>
     </row>
@@ -786,38 +701,33 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1.0</v>
       </c>
       <c r="E36" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G36" s="5">
-        <f>E36*F36</f>
+        <v>0.0</v>
+      </c>
+      <c r="F36" s="5">
+        <f>D36*E36</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="37">
-      <c r="F37" s="2" t="inlineStr">
+      <c r="E37" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G37" s="5">
-        <f>SUM(G35:G36)</f>
+      <c r="F37" s="5">
+        <f>SUM(F35:F36)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -836,30 +746,25 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F40" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G40" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -873,27 +778,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4.0</v>
       </c>
       <c r="E41" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F41" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G41" s="5">
-        <f>E41*F41</f>
+      <c r="F41" s="5">
+        <f>D41*E41</f>
         <v>0.0</v>
       </c>
     </row>
@@ -905,38 +805,33 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1.0</v>
       </c>
       <c r="E42" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G42" s="5">
-        <f>E42*F42</f>
+        <v>0.0</v>
+      </c>
+      <c r="F42" s="5">
+        <f>D42*E42</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="43">
-      <c r="F43" s="2" t="inlineStr">
+      <c r="E43" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G43" s="5">
-        <f>SUM(G41:G42)</f>
+      <c r="F43" s="5">
+        <f>SUM(F41:F42)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -955,30 +850,25 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F46" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G46" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -992,27 +882,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>4.0</v>
       </c>
       <c r="E47" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F47" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G47" s="5">
-        <f>E47*F47</f>
+      <c r="F47" s="5">
+        <f>D47*E47</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1024,38 +909,33 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.0</v>
       </c>
       <c r="E48" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G48" s="5">
-        <f>E48*F48</f>
+        <v>0.0</v>
+      </c>
+      <c r="F48" s="5">
+        <f>D48*E48</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="49">
-      <c r="F49" s="2" t="inlineStr">
+      <c r="E49" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G49" s="5">
-        <f>SUM(G47:G48)</f>
+      <c r="F49" s="5">
+        <f>SUM(F47:F48)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1074,30 +954,25 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F52" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G52" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1111,27 +986,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>4.0</v>
       </c>
       <c r="E53" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F53" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G53" s="5">
-        <f>E53*F53</f>
+      <c r="F53" s="5">
+        <f>D53*E53</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1143,38 +1013,33 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.0</v>
       </c>
       <c r="E54" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G54" s="5">
-        <f>E54*F54</f>
+        <v>0.0</v>
+      </c>
+      <c r="F54" s="5">
+        <f>D54*E54</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="55">
-      <c r="F55" s="2" t="inlineStr">
+      <c r="E55" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G55" s="5">
-        <f>SUM(G53:G54)</f>
+      <c r="F55" s="5">
+        <f>SUM(F53:F54)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1193,30 +1058,25 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F58" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G58" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1230,27 +1090,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>4.0</v>
       </c>
       <c r="E59" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F59" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G59" s="5">
-        <f>E59*F59</f>
+      <c r="F59" s="5">
+        <f>D59*E59</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1262,38 +1117,33 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.0</v>
       </c>
       <c r="E60" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G60" s="5">
-        <f>E60*F60</f>
+        <v>0.0</v>
+      </c>
+      <c r="F60" s="5">
+        <f>D60*E60</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="61">
-      <c r="F61" s="2" t="inlineStr">
+      <c r="E61" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G61" s="5">
-        <f>SUM(G59:G60)</f>
+      <c r="F61" s="5">
+        <f>SUM(F59:F60)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1312,30 +1162,25 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F64" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G64" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1349,27 +1194,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4.0</v>
       </c>
       <c r="E65" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F65" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G65" s="5">
-        <f>E65*F65</f>
+      <c r="F65" s="5">
+        <f>D65*E65</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1381,38 +1221,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.0</v>
       </c>
       <c r="E66" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G66" s="5">
-        <f>E66*F66</f>
+        <v>0.0</v>
+      </c>
+      <c r="F66" s="5">
+        <f>D66*E66</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="67">
-      <c r="F67" s="2" t="inlineStr">
+      <c r="E67" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G67" s="5">
-        <f>SUM(G65:G66)</f>
+      <c r="F67" s="5">
+        <f>SUM(F65:F66)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1431,30 +1266,25 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F70" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G70" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1468,27 +1298,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>4.0</v>
       </c>
       <c r="E71" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F71" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G71" s="5">
-        <f>E71*F71</f>
+      <c r="F71" s="5">
+        <f>D71*E71</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1500,38 +1325,33 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1.0</v>
       </c>
       <c r="E72" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F72" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G72" s="5">
-        <f>E72*F72</f>
+        <v>0.0</v>
+      </c>
+      <c r="F72" s="5">
+        <f>D72*E72</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="F73" s="2" t="inlineStr">
+      <c r="E73" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G73" s="5">
-        <f>SUM(G71:G72)</f>
+      <c r="F73" s="5">
+        <f>SUM(F71:F72)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1550,30 +1370,25 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F76" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G76" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1587,27 +1402,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>4.0</v>
       </c>
       <c r="E77" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F77" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G77" s="5">
-        <f>E77*F77</f>
+      <c r="F77" s="5">
+        <f>D77*E77</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1619,38 +1429,33 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>1.0</v>
       </c>
       <c r="E78" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G78" s="5">
-        <f>E78*F78</f>
+        <v>0.0</v>
+      </c>
+      <c r="F78" s="5">
+        <f>D78*E78</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="79">
-      <c r="F79" s="2" t="inlineStr">
+      <c r="E79" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G79" s="5">
-        <f>SUM(G77:G78)</f>
+      <c r="F79" s="5">
+        <f>SUM(F77:F78)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1669,30 +1474,25 @@
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F82" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G82" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1706,27 +1506,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>4.0</v>
       </c>
       <c r="E83" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F83" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G83" s="5">
-        <f>E83*F83</f>
+      <c r="F83" s="5">
+        <f>D83*E83</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1738,38 +1533,33 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.0</v>
       </c>
       <c r="E84" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F84" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G84" s="5">
-        <f>E84*F84</f>
+        <v>0.0</v>
+      </c>
+      <c r="F84" s="5">
+        <f>D84*E84</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="85">
-      <c r="F85" s="2" t="inlineStr">
+      <c r="E85" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G85" s="5">
-        <f>SUM(G83:G84)</f>
+      <c r="F85" s="5">
+        <f>SUM(F83:F84)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1788,30 +1578,25 @@
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E88" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F88" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G88" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1825,27 +1610,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>4.0</v>
       </c>
       <c r="E89" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F89" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G89" s="5">
-        <f>E89*F89</f>
+      <c r="F89" s="5">
+        <f>D89*E89</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1857,38 +1637,33 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>1.0</v>
       </c>
       <c r="E90" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F90" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G90" s="5">
-        <f>E90*F90</f>
+        <v>0.0</v>
+      </c>
+      <c r="F90" s="5">
+        <f>D90*E90</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="91">
-      <c r="F91" s="2" t="inlineStr">
+      <c r="E91" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G91" s="5">
-        <f>SUM(G89:G90)</f>
+      <c r="F91" s="5">
+        <f>SUM(F89:F90)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1907,30 +1682,25 @@
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F94" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G94" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -1944,27 +1714,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>4.0</v>
       </c>
       <c r="E95" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F95" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G95" s="5">
-        <f>E95*F95</f>
+      <c r="F95" s="5">
+        <f>D95*E95</f>
         <v>0.0</v>
       </c>
     </row>
@@ -1976,38 +1741,33 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>1.0</v>
       </c>
       <c r="E96" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F96" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G96" s="5">
-        <f>E96*F96</f>
+        <v>0.0</v>
+      </c>
+      <c r="F96" s="5">
+        <f>D96*E96</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="97">
-      <c r="F97" s="2" t="inlineStr">
+      <c r="E97" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G97" s="5">
-        <f>SUM(G95:G96)</f>
+      <c r="F97" s="5">
+        <f>SUM(F95:F96)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2026,30 +1786,25 @@
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E100" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F100" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G100" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -2063,27 +1818,22 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>4.0</v>
       </c>
       <c r="E101" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F101" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G101" s="5">
-        <f>E101*F101</f>
+      <c r="F101" s="5">
+        <f>D101*E101</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2095,38 +1845,33 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>1.0</v>
       </c>
       <c r="E102" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F102" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G102" s="5">
-        <f>E102*F102</f>
+        <v>0.0</v>
+      </c>
+      <c r="F102" s="5">
+        <f>D102*E102</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="103">
-      <c r="F103" s="2" t="inlineStr">
+      <c r="E103" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G103" s="5">
-        <f>SUM(G101:G102)</f>
+      <c r="F103" s="5">
+        <f>SUM(F101:F102)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2145,30 +1890,25 @@
       </c>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D106" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E106" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F106" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G106" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -2182,27 +1922,22 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>4.0</v>
       </c>
       <c r="E107" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F107" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G107" s="5">
-        <f>E107*F107</f>
+      <c r="F107" s="5">
+        <f>D107*E107</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2214,38 +1949,33 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1.0</v>
       </c>
       <c r="E108" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F108" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G108" s="5">
-        <f>E108*F108</f>
+        <v>0.0</v>
+      </c>
+      <c r="F108" s="5">
+        <f>D108*E108</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="109">
-      <c r="F109" s="2" t="inlineStr">
+      <c r="E109" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G109" s="5">
-        <f>SUM(G107:G108)</f>
+      <c r="F109" s="5">
+        <f>SUM(F107:F108)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2264,30 +1994,25 @@
       </c>
       <c r="B112" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C112" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D112" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E112" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F112" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G112" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -2301,27 +2026,22 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>4.0</v>
       </c>
       <c r="E113" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F113" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G113" s="5">
-        <f>E113*F113</f>
+      <c r="F113" s="5">
+        <f>D113*E113</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2333,38 +2053,33 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>1.0</v>
       </c>
       <c r="E114" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G114" s="5">
-        <f>E114*F114</f>
+        <v>0.0</v>
+      </c>
+      <c r="F114" s="5">
+        <f>D114*E114</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="115">
-      <c r="F115" s="2" t="inlineStr">
+      <c r="E115" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G115" s="5">
-        <f>SUM(G113:G114)</f>
+      <c r="F115" s="5">
+        <f>SUM(F113:F114)</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2383,30 +2098,25 @@
       </c>
       <c r="B118" s="2" t="inlineStr">
         <is>
-          <t>Contribution type</t>
+          <t>Contributor</t>
         </is>
       </c>
       <c r="C118" s="2" t="inlineStr">
         <is>
-          <t>Contributor</t>
+          <t>Unit type</t>
         </is>
       </c>
       <c r="D118" s="2" t="inlineStr">
         <is>
-          <t>Unit type</t>
+          <t>Unit number</t>
         </is>
       </c>
       <c r="E118" s="2" t="inlineStr">
         <is>
-          <t>Unit number</t>
+          <t>Unit amount</t>
         </is>
       </c>
       <c r="F118" s="2" t="inlineStr">
-        <is>
-          <t>Unit amount</t>
-        </is>
-      </c>
-      <c r="G118" s="2" t="inlineStr">
         <is>
           <t>Total contribution</t>
         </is>
@@ -2420,27 +2130,22 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>4.0</v>
       </c>
       <c r="E119" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="F119" t="n">
         <v>10000.0</v>
       </c>
-      <c r="G119" s="5">
-        <f>E119*F119</f>
+      <c r="F119" s="5">
+        <f>D119*E119</f>
         <v>0.0</v>
       </c>
     </row>
@@ -2452,102 +2157,97 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Central government</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Days</t>
-        </is>
+          <t>Days</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>1.0</v>
       </c>
       <c r="E120" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G120" s="5">
-        <f>E120*F120</f>
+        <v>0.0</v>
+      </c>
+      <c r="F120" s="5">
+        <f>D120*E120</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="121">
-      <c r="F121" s="2" t="inlineStr">
+      <c r="E121" s="2" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="G121" s="5">
-        <f>SUM(G119:G120)</f>
+      <c r="F121" s="5">
+        <f>SUM(F119:F120)</f>
         <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="20">
     <dataValidation type="list" sqref="B5:B6" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B11:B12" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B17:B18" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B23:B24" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B29:B30" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B35:B36" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B41:B42" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B47:B48" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B53:B54" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B59:B60" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B65:B66" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B71:B72" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B77:B78" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B83:B84" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B89:B90" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B95:B96" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B101:B102" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B107:B108" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B113:B114" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="B119:B120" errorStyle="stop" allowBlank="true" showErrorMessage="true">
-      <formula1>"Central government,Local government,Local NGO,International NGO,Other,Beneficiaries"</formula1>
+      <formula1>"Not specified,Public/state resources,a,,b"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>